<commit_message>
added note for RF lower cutoff
</commit_message>
<xml_diff>
--- a/data/Model_Comparison_Matrix.xlsx
+++ b/data/Model_Comparison_Matrix.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/383c7e8e9c1613b5/Documents/MSDS6372/Proj2/stats2proj2/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carol\OneDrive\Documents\MSDS6372\Proj2\stats2proj2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="57" documentId="8_{EC295531-0FB2-4DBF-BEB6-ACBE5728803E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{3176A616-35B6-4EF5-AEA3-A8FB890F1F5B}"/>
+  <xr:revisionPtr revIDLastSave="63" documentId="8_{EC295531-0FB2-4DBF-BEB6-ACBE5728803E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{B69AE127-28BE-4174-9725-854B70168679}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8430" xr2:uid="{AE95EDD6-F72B-4BDD-9720-396E5E427100}"/>
   </bookViews>
@@ -63,9 +63,6 @@
     <t>(67.4%, 81.9%)</t>
   </si>
   <si>
-    <t>Random Forest</t>
-  </si>
-  <si>
     <t>(66%, 80.7%)</t>
   </si>
   <si>
@@ -78,7 +75,10 @@
     <t>(65.3%, 80.1%)</t>
   </si>
   <si>
-    <t>RF Lower Cutoff</t>
+    <t>Random Forest*</t>
+  </si>
+  <si>
+    <t>*RF Lower Cutoff (decreasing the probability from 50% to 30%)</t>
   </si>
 </sst>
 </file>
@@ -187,22 +187,6 @@
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="9">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Simplified Arabic Fixed"/>
-        <family val="3"/>
-        <charset val="178"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -346,6 +330,22 @@
         <charset val="178"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Simplified Arabic Fixed"/>
+        <family val="3"/>
+        <charset val="178"/>
+        <scheme val="none"/>
+      </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
@@ -362,16 +362,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DDC1AA50-EF39-4817-9F0C-FC0A1823EE55}" name="Table1" displayName="Table1" ref="A1:G7" totalsRowShown="0" headerRowDxfId="8" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DDC1AA50-EF39-4817-9F0C-FC0A1823EE55}" name="Table1" displayName="Table1" ref="A1:G7" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="A1:G7" xr:uid="{B1A6DFC8-6989-47AF-910A-49921DE8B32F}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{556D222C-B1A5-4536-A2D8-DA25D823ACB0}" name="Model" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{3BE4A022-D5F6-4462-91FC-231F7C5AD026}" name="Predictors" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{557B2F62-87D7-4D40-ADAD-064CED992F56}" name="Accuracy" dataDxfId="5" dataCellStyle="Percent"/>
-    <tableColumn id="4" xr3:uid="{4D37E08E-42FB-4F11-800F-C1767BC0BF2B}" name="95% CI" dataDxfId="4" dataCellStyle="Percent"/>
-    <tableColumn id="5" xr3:uid="{370F81C5-FDC8-4799-8666-B7F48788627A}" name="Sensitivity" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{59A955DD-BC64-4115-BB73-9C6B648C8B47}" name="Specificity" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{542ECED0-300D-4E03-9C31-AF7F170A95E3}" name="AUC" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{556D222C-B1A5-4536-A2D8-DA25D823ACB0}" name="Model" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{3BE4A022-D5F6-4462-91FC-231F7C5AD026}" name="Predictors" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{557B2F62-87D7-4D40-ADAD-064CED992F56}" name="Accuracy" dataDxfId="4" dataCellStyle="Percent"/>
+    <tableColumn id="4" xr3:uid="{4D37E08E-42FB-4F11-800F-C1767BC0BF2B}" name="95% CI" dataDxfId="3" dataCellStyle="Percent"/>
+    <tableColumn id="5" xr3:uid="{370F81C5-FDC8-4799-8666-B7F48788627A}" name="Sensitivity" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{59A955DD-BC64-4115-BB73-9C6B648C8B47}" name="Specificity" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{542ECED0-300D-4E03-9C31-AF7F170A95E3}" name="AUC" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -677,12 +677,12 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="34.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="43" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.140625" style="2" customWidth="1"/>
     <col min="3" max="3" width="18.140625" style="3" customWidth="1"/>
     <col min="4" max="4" width="25.140625" style="3" customWidth="1"/>
@@ -762,7 +762,7 @@
     </row>
     <row r="4" spans="1:7" s="11" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B4" s="9">
         <v>10</v>
@@ -783,7 +783,7 @@
         <v>0.74199999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="11" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="11" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>17</v>
       </c>
@@ -794,7 +794,7 @@
         <v>0.73829999999999996</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5" s="12">
         <v>0.91069999999999995</v>
@@ -806,7 +806,7 @@
     </row>
     <row r="6" spans="1:7" s="11" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="9">
         <v>10</v>
@@ -829,7 +829,7 @@
     </row>
     <row r="7" spans="1:7" s="11" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="9">
         <v>4</v>
@@ -838,7 +838,7 @@
         <v>0.73150000000000004</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E7" s="12">
         <v>0.94642999999999999</v>

</xml_diff>